<commit_message>
LAP22G33-115 US301 UCD, MD and SSD
</commit_message>
<xml_diff>
--- a/LAPR3-2021-Self-Assessment.xlsx
+++ b/LAPR3-2021-Self-Assessment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\IdeaProjects\lapr3-2021-g033\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2EB00C2-6387-40CF-8367-C03F97A14DBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5DD8A04-813C-4325-92CB-0AF550EE68D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{5ECC33D7-267E-3941-AADB-18CFA00ADDCE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5ECC33D7-267E-3941-AADB-18CFA00ADDCE}"/>
   </bookViews>
   <sheets>
     <sheet name="Group and Self Assessment" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="165">
   <si>
     <t>Fill the cells with a blue background</t>
   </si>
@@ -194,43 +194,13 @@
     <t>The students have exceeded expectations </t>
   </si>
   <si>
-    <t>US101</t>
-  </si>
-  <si>
     <t>The students  have exceeded expectations </t>
   </si>
   <si>
-    <t>US102</t>
-  </si>
-  <si>
-    <t>US103</t>
-  </si>
-  <si>
-    <t>US104</t>
-  </si>
-  <si>
-    <t>US105</t>
-  </si>
-  <si>
-    <t>US106</t>
-  </si>
-  <si>
     <t>US107</t>
   </si>
   <si>
-    <t>US108</t>
-  </si>
-  <si>
-    <t>US109</t>
-  </si>
-  <si>
-    <t>US110</t>
-  </si>
-  <si>
     <t>US111</t>
-  </si>
-  <si>
-    <t>US112</t>
   </si>
   <si>
     <t>Code Quality based on Sonarqube Data</t>
@@ -580,7 +550,34 @@
     <t>LAPR3 Project Group and Self-assessment v1.0</t>
   </si>
   <si>
-    <t>Originaly of 1200546</t>
+    <t>US201</t>
+  </si>
+  <si>
+    <t>US202</t>
+  </si>
+  <si>
+    <t>US203</t>
+  </si>
+  <si>
+    <t>US204</t>
+  </si>
+  <si>
+    <t>US205</t>
+  </si>
+  <si>
+    <t>US206</t>
+  </si>
+  <si>
+    <t>US207</t>
+  </si>
+  <si>
+    <t>US208</t>
+  </si>
+  <si>
+    <t>US209</t>
+  </si>
+  <si>
+    <t>US210</t>
   </si>
 </sst>
 </file>
@@ -2085,8 +2082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A51149F-37F8-9041-812D-F0949B9CB00F}">
   <dimension ref="A1:T36"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2099,7 +2096,7 @@
   <sheetData>
     <row r="1" spans="1:20" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2119,7 +2116,9 @@
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="6"/>
+      <c r="B4" s="6">
+        <v>33</v>
+      </c>
       <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
@@ -2227,16 +2226,16 @@
         <v>1201237</v>
       </c>
       <c r="D10" s="39">
+        <v>5</v>
+      </c>
+      <c r="E10" s="41">
+        <v>5</v>
+      </c>
+      <c r="F10" s="42">
         <v>4</v>
       </c>
-      <c r="E10" s="41">
+      <c r="G10" s="42">
         <v>4</v>
-      </c>
-      <c r="F10" s="42">
-        <v>3</v>
-      </c>
-      <c r="G10" s="42">
-        <v>2</v>
       </c>
       <c r="H10" s="42"/>
       <c r="I10" s="42"/>
@@ -2251,7 +2250,7 @@
       <c r="R10" s="40"/>
       <c r="S10" s="53">
         <f>AVERAGE(D10:R10)</f>
-        <v>3.25</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="11" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2260,16 +2259,16 @@
         <v>1201274</v>
       </c>
       <c r="D11" s="9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E11" s="39">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F11" s="38">
         <v>4</v>
       </c>
       <c r="G11" s="8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H11" s="8"/>
       <c r="I11" s="8"/>
@@ -2284,7 +2283,7 @@
       <c r="R11" s="10"/>
       <c r="S11" s="54">
         <f t="shared" ref="S11:S24" si="0">AVERAGE(D11:R11)</f>
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2293,16 +2292,16 @@
         <v>1190772</v>
       </c>
       <c r="D12" s="8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E12" s="9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F12" s="39">
         <v>4</v>
       </c>
       <c r="G12" s="38">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
@@ -2317,7 +2316,7 @@
       <c r="R12" s="10"/>
       <c r="S12" s="54">
         <f t="shared" si="0"/>
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="13" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2332,10 +2331,10 @@
         <v>5</v>
       </c>
       <c r="F13" s="9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G13" s="39">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H13" s="38"/>
       <c r="I13" s="8"/>
@@ -2350,7 +2349,7 @@
       <c r="R13" s="10"/>
       <c r="S13" s="54">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>4.25</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2635,11 +2634,11 @@
       </c>
       <c r="D25" s="49">
         <f>AVERAGE(D10:D24)</f>
-        <v>4.25</v>
+        <v>5</v>
       </c>
       <c r="E25" s="49">
         <f t="shared" ref="E25:R25" si="1">AVERAGE(E10:E24)</f>
-        <v>4.25</v>
+        <v>5</v>
       </c>
       <c r="F25" s="49">
         <f t="shared" si="1"/>
@@ -2647,7 +2646,7 @@
       </c>
       <c r="G25" s="49">
         <f t="shared" si="1"/>
-        <v>1.75</v>
+        <v>3.75</v>
       </c>
       <c r="H25" s="49" t="e">
         <f t="shared" si="1"/>
@@ -2782,8 +2781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{049E9D47-BAA1-5945-9716-C25FEE03B60C}">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2882,13 +2881,13 @@
     </row>
     <row r="6" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B6" s="8">
-        <v>1190772</v>
+        <v>1201237</v>
       </c>
       <c r="C6" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D6" s="13"/>
       <c r="E6" s="34" t="s">
@@ -2907,12 +2906,12 @@
         <v>43</v>
       </c>
       <c r="J6" s="36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>47</v>
+        <v>155</v>
       </c>
       <c r="B7" s="8">
         <v>1201237</v>
@@ -2937,15 +2936,15 @@
         <v>43</v>
       </c>
       <c r="J7" s="36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>48</v>
+        <v>156</v>
       </c>
       <c r="B8" s="8">
-        <v>1201237</v>
+        <v>1201274</v>
       </c>
       <c r="C8" s="8">
         <v>4</v>
@@ -2967,18 +2966,18 @@
         <v>43</v>
       </c>
       <c r="J8" s="36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>49</v>
+        <v>157</v>
       </c>
       <c r="B9" s="8">
-        <v>1201274</v>
+        <v>1201237</v>
       </c>
       <c r="C9" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D9" s="13"/>
       <c r="E9" s="15" t="s">
@@ -2997,12 +2996,12 @@
         <v>43</v>
       </c>
       <c r="J9" s="36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>50</v>
+        <v>158</v>
       </c>
       <c r="B10" s="8">
         <v>1201274</v>
@@ -3010,9 +3009,7 @@
       <c r="C10" s="8">
         <v>4</v>
       </c>
-      <c r="D10" s="13" t="s">
-        <v>165</v>
-      </c>
+      <c r="D10" s="13"/>
       <c r="E10" s="15" t="s">
         <v>39</v>
       </c>
@@ -3029,18 +3026,18 @@
         <v>43</v>
       </c>
       <c r="J10" s="36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>51</v>
+        <v>159</v>
       </c>
       <c r="B11" s="8">
-        <v>1190772</v>
+        <v>1200546</v>
       </c>
       <c r="C11" s="8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D11" s="13"/>
       <c r="E11" s="15" t="s">
@@ -3059,18 +3056,18 @@
         <v>43</v>
       </c>
       <c r="J11" s="36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>52</v>
+        <v>160</v>
       </c>
       <c r="B12" s="8">
         <v>1200546</v>
       </c>
       <c r="C12" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" s="13"/>
       <c r="E12" s="15" t="s">
@@ -3089,12 +3086,12 @@
         <v>43</v>
       </c>
       <c r="J12" s="36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>53</v>
+        <v>161</v>
       </c>
       <c r="B13" s="8">
         <v>1201274</v>
@@ -3119,15 +3116,15 @@
         <v>43</v>
       </c>
       <c r="J13" s="36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>54</v>
+        <v>162</v>
       </c>
       <c r="B14" s="8">
-        <v>1201237</v>
+        <v>1190772</v>
       </c>
       <c r="C14" s="8">
         <v>4</v>
@@ -3149,12 +3146,12 @@
         <v>43</v>
       </c>
       <c r="J14" s="36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>55</v>
+        <v>163</v>
       </c>
       <c r="B15" s="8">
         <v>1190772</v>
@@ -3179,18 +3176,18 @@
         <v>43</v>
       </c>
       <c r="J15" s="36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>56</v>
+        <v>164</v>
       </c>
       <c r="B16" s="8">
-        <v>1200546</v>
+        <v>1201274</v>
       </c>
       <c r="C16" s="8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D16" s="13"/>
       <c r="E16" s="15" t="s">
@@ -3209,15 +3206,19 @@
         <v>43</v>
       </c>
       <c r="J16" s="36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
+        <v>47</v>
+      </c>
+      <c r="B17" s="8">
+        <v>1200546</v>
+      </c>
+      <c r="C17" s="8">
+        <v>4</v>
+      </c>
       <c r="D17" s="13"/>
       <c r="E17" s="15" t="s">
         <v>39</v>
@@ -3235,7 +3236,7 @@
         <v>43</v>
       </c>
       <c r="J17" s="36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
@@ -3259,7 +3260,7 @@
         <v>43</v>
       </c>
       <c r="J18" s="36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
@@ -3283,7 +3284,7 @@
         <v>43</v>
       </c>
       <c r="J19" s="36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
@@ -3307,7 +3308,7 @@
         <v>43</v>
       </c>
       <c r="J20" s="36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
@@ -3331,7 +3332,7 @@
         <v>43</v>
       </c>
       <c r="J21" s="36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
@@ -3355,7 +3356,7 @@
         <v>43</v>
       </c>
       <c r="J22" s="36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
@@ -3379,7 +3380,7 @@
         <v>43</v>
       </c>
       <c r="J23" s="36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
@@ -3403,7 +3404,7 @@
         <v>43</v>
       </c>
       <c r="J24" s="36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="48" thickBot="1" x14ac:dyDescent="0.3">
@@ -3427,7 +3428,7 @@
         <v>43</v>
       </c>
       <c r="J25" s="36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -3550,8 +3551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59B77AED-41D5-8047-A901-AF6E531ADCF8}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3562,39 +3563,39 @@
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="33" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:6" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="60" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B3" s="59" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C3" s="57" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="D3" s="57" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="E3" s="57" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="F3" s="58" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="61" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="B4" s="11">
         <v>34</v>
       </c>
       <c r="C4" s="64">
-        <v>88.5</v>
+        <v>83.9</v>
       </c>
       <c r="D4" s="22">
         <v>80</v>
@@ -3604,39 +3605,39 @@
       </c>
       <c r="F4" s="12">
         <f>IF(((C4-D4)/(E4-D4)*100)&gt;100,100,(C4-D4)/(E4-D4)*100)</f>
-        <v>85</v>
+        <v>39.000000000000057</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="62" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B5" s="15">
         <v>21</v>
       </c>
       <c r="C5" s="31">
-        <v>75.900000000000006</v>
+        <v>73.900000000000006</v>
       </c>
       <c r="D5" s="7">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="E5" s="7">
         <v>85</v>
       </c>
       <c r="F5" s="16">
         <f>IF(((C5-D5)/(E5-D5)*100)&gt;100,100,(C5-D5)/(E5-D5)*100)</f>
-        <v>9.0000000000000568</v>
+        <v>44.500000000000028</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="62" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="B6" s="15">
         <v>-13</v>
       </c>
       <c r="C6" s="30">
-        <v>1.2</v>
+        <v>0.9</v>
       </c>
       <c r="D6" s="7">
         <v>5</v>
@@ -3651,7 +3652,7 @@
     </row>
     <row r="7" spans="1:6" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="63" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="B7" s="23">
         <v>-13</v>
@@ -3672,7 +3673,7 @@
     </row>
     <row r="8" spans="1:6" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="48" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B8" s="57">
         <v>55</v>
@@ -3682,7 +3683,7 @@
       <c r="E8" s="57"/>
       <c r="F8" s="58">
         <f>SUMPRODUCT(B4:B7,F4:F7)/100</f>
-        <v>30.790000000000013</v>
+        <v>22.605000000000022</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3691,11 +3692,11 @@
       <c r="C9" s="67"/>
       <c r="D9" s="68"/>
       <c r="E9" s="48" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="F9" s="69">
         <f>IF((F8/B8)&lt;0,0,(F8/B8))</f>
-        <v>0.5598181818181821</v>
+        <v>0.41100000000000042</v>
       </c>
     </row>
   </sheetData>
@@ -3708,7 +3709,7 @@
   <dimension ref="A1:Z11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3730,7 +3731,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
@@ -3750,10 +3751,10 @@
     <row r="2" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:26" ht="57" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C3" s="21">
         <f>'Group and Self Assessment'!C10</f>
@@ -3843,7 +3844,7 @@
         <v>5</v>
       </c>
       <c r="Y3" s="22" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="Z3" s="12" t="s">
         <v>32</v>
@@ -3851,99 +3852,99 @@
     </row>
     <row r="4" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="B4" s="18">
         <v>0.35</v>
       </c>
       <c r="C4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>2.7990909090909106</v>
+        <v>2.0550000000000019</v>
       </c>
       <c r="D4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>2.7990909090909106</v>
+        <v>2.0550000000000019</v>
       </c>
       <c r="E4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>2.7990909090909106</v>
+        <v>2.0550000000000019</v>
       </c>
       <c r="F4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>2.7990909090909106</v>
+        <v>2.0550000000000019</v>
       </c>
       <c r="G4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>2.7990909090909106</v>
+        <v>2.0550000000000019</v>
       </c>
       <c r="H4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>2.7990909090909106</v>
+        <v>2.0550000000000019</v>
       </c>
       <c r="I4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>2.7990909090909106</v>
+        <v>2.0550000000000019</v>
       </c>
       <c r="J4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>2.7990909090909106</v>
+        <v>2.0550000000000019</v>
       </c>
       <c r="K4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>2.7990909090909106</v>
+        <v>2.0550000000000019</v>
       </c>
       <c r="L4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>2.7990909090909106</v>
+        <v>2.0550000000000019</v>
       </c>
       <c r="M4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>2.7990909090909106</v>
+        <v>2.0550000000000019</v>
       </c>
       <c r="N4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>2.7990909090909106</v>
+        <v>2.0550000000000019</v>
       </c>
       <c r="O4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>2.7990909090909106</v>
+        <v>2.0550000000000019</v>
       </c>
       <c r="P4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>2.7990909090909106</v>
+        <v>2.0550000000000019</v>
       </c>
       <c r="Q4" s="32">
         <f>'Code Quality'!$F$9*5</f>
-        <v>2.7990909090909106</v>
+        <v>2.0550000000000019</v>
       </c>
       <c r="R4" s="28">
         <f>AVERAGE(C4:Q4)</f>
-        <v>2.7990909090909097</v>
+        <v>2.0550000000000024</v>
       </c>
       <c r="S4" s="7" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="T4" s="7" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="U4" s="7" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="V4" s="7" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="W4" s="7" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="X4" s="7" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="Y4" s="7"/>
       <c r="Z4" s="16"/>
     </row>
     <row r="5" spans="1:26" ht="63" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B5" s="18">
         <v>7.4999999999999997E-2</v>
@@ -3958,7 +3959,7 @@
         <v>3</v>
       </c>
       <c r="F5" s="26">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G5" s="26"/>
       <c r="H5" s="26"/>
@@ -3973,32 +3974,32 @@
       <c r="Q5" s="26"/>
       <c r="R5" s="28">
         <f t="shared" ref="R5:R8" si="0">AVERAGE(C5:Q5)</f>
-        <v>2.5</v>
+        <v>3.25</v>
       </c>
       <c r="S5" s="7" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="T5" s="7" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="U5" s="7" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="V5" s="7" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="W5" s="7" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="X5" s="7" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="Y5" s="7"/>
       <c r="Z5" s="16"/>
     </row>
     <row r="6" spans="1:26" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="B6" s="18">
         <v>0.1</v>
@@ -4007,13 +4008,13 @@
         <v>4</v>
       </c>
       <c r="D6" s="26">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E6" s="26">
         <v>3</v>
       </c>
       <c r="F6" s="26">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G6" s="26"/>
       <c r="H6" s="26"/>
@@ -4028,32 +4029,32 @@
       <c r="Q6" s="26"/>
       <c r="R6" s="28">
         <f t="shared" si="0"/>
-        <v>2.75</v>
+        <v>3.25</v>
       </c>
       <c r="S6" s="7" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="T6" s="7" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="U6" s="7" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="V6" s="7" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="W6" s="7" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="X6" s="7" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="Y6" s="7"/>
       <c r="Z6" s="16"/>
     </row>
     <row r="7" spans="1:26" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="B7" s="18">
         <v>0.35</v>
@@ -4062,13 +4063,13 @@
         <v>4</v>
       </c>
       <c r="D7" s="26">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E7" s="26">
         <v>3</v>
       </c>
       <c r="F7" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" s="26"/>
       <c r="H7" s="26"/>
@@ -4086,29 +4087,29 @@
         <v>2.5</v>
       </c>
       <c r="S7" s="7" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="T7" s="7" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="U7" s="7" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="V7" s="7" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="W7" s="7" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="X7" s="7" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="Y7" s="7"/>
       <c r="Z7" s="16"/>
     </row>
     <row r="8" spans="1:26" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="B8" s="18">
         <v>0.125</v>
@@ -4123,7 +4124,7 @@
         <v>4</v>
       </c>
       <c r="F8" s="26">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G8" s="26"/>
       <c r="H8" s="26"/>
@@ -4138,32 +4139,32 @@
       <c r="Q8" s="26"/>
       <c r="R8" s="28">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S8" s="7" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="T8" s="7" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="U8" s="7" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="V8" s="7" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="W8" s="7" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="X8" s="7" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="Y8" s="7"/>
       <c r="Z8" s="16"/>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B9" s="19">
         <f>SUM(B4:B8)</f>
@@ -4171,63 +4172,63 @@
       </c>
       <c r="C9" s="7">
         <f>SUMPRODUCT(C4:C8,$B$4:$B$8)</f>
-        <v>3.5796818181818186</v>
+        <v>3.3192500000000007</v>
       </c>
       <c r="D9" s="7">
         <f t="shared" ref="D9:Q9" si="1">SUMPRODUCT(D4:D8,$B$4:$B$8)</f>
-        <v>3.1546818181818184</v>
+        <v>2.4442500000000003</v>
       </c>
       <c r="E9" s="7">
         <f t="shared" si="1"/>
-        <v>3.0546818181818187</v>
+        <v>2.7942500000000003</v>
       </c>
       <c r="F9" s="7">
         <f t="shared" si="1"/>
-        <v>0.97968181818181865</v>
+        <v>2.0942500000000006</v>
       </c>
       <c r="G9" s="7">
         <f t="shared" si="1"/>
-        <v>0.97968181818181865</v>
+        <v>0.71925000000000061</v>
       </c>
       <c r="H9" s="7">
         <f t="shared" si="1"/>
-        <v>0.97968181818181865</v>
+        <v>0.71925000000000061</v>
       </c>
       <c r="I9" s="7">
         <f t="shared" si="1"/>
-        <v>0.97968181818181865</v>
+        <v>0.71925000000000061</v>
       </c>
       <c r="J9" s="7">
         <f t="shared" si="1"/>
-        <v>0.97968181818181865</v>
+        <v>0.71925000000000061</v>
       </c>
       <c r="K9" s="7">
         <f t="shared" si="1"/>
-        <v>0.97968181818181865</v>
+        <v>0.71925000000000061</v>
       </c>
       <c r="L9" s="7">
         <f t="shared" si="1"/>
-        <v>0.97968181818181865</v>
+        <v>0.71925000000000061</v>
       </c>
       <c r="M9" s="7">
         <f t="shared" si="1"/>
-        <v>0.97968181818181865</v>
+        <v>0.71925000000000061</v>
       </c>
       <c r="N9" s="7">
         <f t="shared" si="1"/>
-        <v>0.97968181818181865</v>
+        <v>0.71925000000000061</v>
       </c>
       <c r="O9" s="7">
         <f t="shared" si="1"/>
-        <v>0.97968181818181865</v>
+        <v>0.71925000000000061</v>
       </c>
       <c r="P9" s="7">
         <f t="shared" si="1"/>
-        <v>0.97968181818181865</v>
+        <v>0.71925000000000061</v>
       </c>
       <c r="Q9" s="7">
         <f t="shared" si="1"/>
-        <v>0.97968181818181865</v>
+        <v>0.71925000000000061</v>
       </c>
       <c r="R9" s="28"/>
       <c r="S9" s="7"/>
@@ -4241,68 +4242,68 @@
     </row>
     <row r="10" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="23" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="B10" s="24"/>
       <c r="C10" s="24">
         <f>C9/5*20</f>
-        <v>14.318727272727275</v>
+        <v>13.277000000000003</v>
       </c>
       <c r="D10" s="24">
         <f t="shared" ref="D10:Q10" si="2">D9/5*20</f>
-        <v>12.618727272727273</v>
+        <v>9.777000000000001</v>
       </c>
       <c r="E10" s="24">
         <f t="shared" si="2"/>
-        <v>12.218727272727275</v>
+        <v>11.177000000000001</v>
       </c>
       <c r="F10" s="24">
         <f t="shared" si="2"/>
-        <v>3.9187272727272751</v>
+        <v>8.3770000000000024</v>
       </c>
       <c r="G10" s="24">
         <f t="shared" si="2"/>
-        <v>3.9187272727272751</v>
+        <v>2.8770000000000024</v>
       </c>
       <c r="H10" s="24">
         <f t="shared" si="2"/>
-        <v>3.9187272727272751</v>
+        <v>2.8770000000000024</v>
       </c>
       <c r="I10" s="24">
         <f t="shared" si="2"/>
-        <v>3.9187272727272751</v>
+        <v>2.8770000000000024</v>
       </c>
       <c r="J10" s="24">
         <f t="shared" si="2"/>
-        <v>3.9187272727272751</v>
+        <v>2.8770000000000024</v>
       </c>
       <c r="K10" s="24">
         <f t="shared" si="2"/>
-        <v>3.9187272727272751</v>
+        <v>2.8770000000000024</v>
       </c>
       <c r="L10" s="24">
         <f t="shared" si="2"/>
-        <v>3.9187272727272751</v>
+        <v>2.8770000000000024</v>
       </c>
       <c r="M10" s="24">
         <f t="shared" si="2"/>
-        <v>3.9187272727272751</v>
+        <v>2.8770000000000024</v>
       </c>
       <c r="N10" s="24">
         <f t="shared" si="2"/>
-        <v>3.9187272727272751</v>
+        <v>2.8770000000000024</v>
       </c>
       <c r="O10" s="24">
         <f t="shared" si="2"/>
-        <v>3.9187272727272751</v>
+        <v>2.8770000000000024</v>
       </c>
       <c r="P10" s="24">
         <f t="shared" si="2"/>
-        <v>3.9187272727272751</v>
+        <v>2.8770000000000024</v>
       </c>
       <c r="Q10" s="24">
         <f t="shared" si="2"/>
-        <v>3.9187272727272751</v>
+        <v>2.8770000000000024</v>
       </c>
       <c r="R10" s="29"/>
       <c r="S10" s="24"/>
@@ -4316,7 +4317,7 @@
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -4334,8 +4335,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C190218-096C-D04F-B5E6-6BE0B32B2632}">
   <dimension ref="A1:Z17"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4355,7 +4356,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="14"/>
@@ -4374,10 +4375,10 @@
     </row>
     <row r="3" spans="1:26" ht="57" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C3" s="21">
         <f>'Group and Self Assessment'!C10</f>
@@ -4467,7 +4468,7 @@
         <v>5</v>
       </c>
       <c r="Y3" s="22" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="Z3" s="12" t="s">
         <v>32</v>
@@ -4475,7 +4476,7 @@
     </row>
     <row r="4" spans="1:26" ht="144.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="B4" s="18">
         <v>0.1</v>
@@ -4508,29 +4509,29 @@
         <v>3</v>
       </c>
       <c r="S4" s="74" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="T4" s="74" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="U4" s="74" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="V4" s="74" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="W4" s="74" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="X4" s="74" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="Y4" s="71"/>
       <c r="Z4" s="16"/>
     </row>
     <row r="5" spans="1:26" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="B5" s="18">
         <v>0.1</v>
@@ -4539,13 +4540,13 @@
         <v>3</v>
       </c>
       <c r="D5" s="26">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E5" s="26">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F5" s="26">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G5" s="26"/>
       <c r="H5" s="26"/>
@@ -4560,32 +4561,32 @@
       <c r="Q5" s="26"/>
       <c r="R5" s="70">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2.25</v>
       </c>
       <c r="S5" s="74" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="T5" s="74" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="U5" s="74" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="V5" s="74" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="W5" s="74" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="X5" s="74" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="Y5" s="71"/>
       <c r="Z5" s="16"/>
     </row>
     <row r="6" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="B6" s="18">
         <v>0.05</v>
@@ -4618,44 +4619,44 @@
         <v>1</v>
       </c>
       <c r="S6" s="74" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="T6" s="74" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="U6" s="74" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="V6" s="74" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="W6" s="74" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="X6" s="74" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="Y6" s="71"/>
       <c r="Z6" s="16"/>
     </row>
     <row r="7" spans="1:26" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="B7" s="18">
         <v>0.05</v>
       </c>
       <c r="C7" s="26">
+        <v>4</v>
+      </c>
+      <c r="D7" s="26">
+        <v>4</v>
+      </c>
+      <c r="E7" s="26">
+        <v>3</v>
+      </c>
+      <c r="F7" s="26">
         <v>1</v>
-      </c>
-      <c r="D7" s="26">
-        <v>0</v>
-      </c>
-      <c r="E7" s="26">
-        <v>0</v>
-      </c>
-      <c r="F7" s="26">
-        <v>0</v>
       </c>
       <c r="G7" s="26"/>
       <c r="H7" s="26"/>
@@ -4670,32 +4671,32 @@
       <c r="Q7" s="26"/>
       <c r="R7" s="70">
         <f t="shared" si="0"/>
-        <v>0.25</v>
+        <v>3</v>
       </c>
       <c r="S7" s="74" t="s">
+        <v>109</v>
+      </c>
+      <c r="T7" s="74" t="s">
+        <v>116</v>
+      </c>
+      <c r="U7" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="V7" s="74" t="s">
+        <v>118</v>
+      </c>
+      <c r="W7" s="74" t="s">
         <v>119</v>
       </c>
-      <c r="T7" s="74" t="s">
-        <v>126</v>
-      </c>
-      <c r="U7" s="74" t="s">
-        <v>127</v>
-      </c>
-      <c r="V7" s="74" t="s">
-        <v>128</v>
-      </c>
-      <c r="W7" s="74" t="s">
-        <v>129</v>
-      </c>
       <c r="X7" s="74" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="Y7" s="71"/>
       <c r="Z7" s="16"/>
     </row>
     <row r="8" spans="1:26" ht="63" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="B8" s="18">
         <v>0.1</v>
@@ -4728,29 +4729,29 @@
         <v>0</v>
       </c>
       <c r="S8" s="74" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="T8" s="74" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="U8" s="74" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="V8" s="74" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="W8" s="74" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="X8" s="74" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="Y8" s="71"/>
       <c r="Z8" s="16"/>
     </row>
     <row r="9" spans="1:26" ht="63" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="B9" s="18">
         <v>0.05</v>
@@ -4759,13 +4760,13 @@
         <v>5</v>
       </c>
       <c r="D9" s="26">
+        <v>5</v>
+      </c>
+      <c r="E9" s="26">
         <v>3</v>
       </c>
-      <c r="E9" s="26">
+      <c r="F9" s="26">
         <v>2</v>
-      </c>
-      <c r="F9" s="26">
-        <v>0</v>
       </c>
       <c r="G9" s="26"/>
       <c r="H9" s="26"/>
@@ -4780,28 +4781,28 @@
       <c r="Q9" s="26"/>
       <c r="R9" s="70">
         <f t="shared" ref="R9:R11" si="2">AVERAGE(C9:Q9)</f>
-        <v>2.5</v>
+        <v>3.75</v>
       </c>
       <c r="S9" s="74" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="T9" s="74" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="U9" s="74"/>
       <c r="V9" s="74" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="W9" s="74"/>
       <c r="X9" s="74" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="Y9" s="71"/>
       <c r="Z9" s="16"/>
     </row>
     <row r="10" spans="1:26" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="B10" s="18">
         <v>0.1</v>
@@ -4834,44 +4835,44 @@
         <v>4</v>
       </c>
       <c r="S10" s="74" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="T10" s="74" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="U10" s="74" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="V10" s="74" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="W10" s="74" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="X10" s="74" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="Y10" s="71"/>
       <c r="Z10" s="16"/>
     </row>
     <row r="11" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="B11" s="18">
         <v>0.1</v>
       </c>
       <c r="C11" s="26">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D11" s="26">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E11" s="26">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F11" s="26">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G11" s="26"/>
       <c r="H11" s="26"/>
@@ -4886,32 +4887,32 @@
       <c r="Q11" s="26"/>
       <c r="R11" s="70">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S11" s="74" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="T11" s="74" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="U11" s="74" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="V11" s="74" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="W11" s="74" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="X11" s="74" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="Y11" s="71"/>
       <c r="Z11" s="16"/>
     </row>
     <row r="12" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="B12" s="18">
         <v>0.1</v>
@@ -4944,29 +4945,29 @@
         <v>4</v>
       </c>
       <c r="S12" s="74" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="T12" s="74" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="U12" s="74" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="V12" s="74" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="W12" s="74" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="X12" s="74" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="Y12" s="71"/>
       <c r="Z12" s="16"/>
     </row>
     <row r="13" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="B13" s="18">
         <v>0.1</v>
@@ -4978,10 +4979,10 @@
         <v>5</v>
       </c>
       <c r="E13" s="26">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F13" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13" s="26"/>
       <c r="H13" s="26"/>
@@ -4996,32 +4997,32 @@
       <c r="Q13" s="26"/>
       <c r="R13" s="70">
         <f t="shared" ref="R13:R14" si="3">AVERAGE(C13:Q13)</f>
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="S13" s="74" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="T13" s="74" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="U13" s="74" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="V13" s="74" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="W13" s="74" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="X13" s="74" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="Y13" s="71"/>
       <c r="Z13" s="16"/>
     </row>
     <row r="14" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="B14" s="18">
         <v>0.15</v>
@@ -5054,29 +5055,29 @@
         <v>3</v>
       </c>
       <c r="S14" s="74" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="T14" s="74" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="U14" s="74" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="V14" s="74" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="W14" s="74" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="X14" s="74" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="Y14" s="71"/>
       <c r="Z14" s="16"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B15" s="19">
         <f>SUM(B4:B14)</f>
@@ -5084,19 +5085,19 @@
       </c>
       <c r="C15" s="7">
         <f t="shared" ref="C15:Q15" si="4">SUMPRODUCT(C8:C14,$B$8:$B$14)</f>
-        <v>2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="D15" s="7">
         <f t="shared" si="4"/>
-        <v>1.9000000000000001</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E15" s="7">
         <f t="shared" si="4"/>
-        <v>1.75</v>
+        <v>2.0999999999999996</v>
       </c>
       <c r="F15" s="7">
         <f t="shared" si="4"/>
-        <v>1.25</v>
+        <v>1.6500000000000001</v>
       </c>
       <c r="G15" s="7">
         <f t="shared" si="4"/>
@@ -5154,24 +5155,24 @@
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="23" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="B16" s="24"/>
       <c r="C16" s="24">
         <f>C15/5*20</f>
-        <v>8</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="D16" s="24">
         <f t="shared" ref="D16:Q16" si="5">D15/5*20</f>
-        <v>7.6</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="E16" s="24">
         <f t="shared" si="5"/>
-        <v>7</v>
+        <v>8.3999999999999986</v>
       </c>
       <c r="F16" s="24">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>6.6000000000000005</v>
       </c>
       <c r="G16" s="24">
         <f t="shared" si="5"/>
@@ -5229,7 +5230,7 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -5440,18 +5441,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5473,6 +5474,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F61419B8-A98A-41CD-95EE-48A4F975B8D1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8D82CB-2E6F-4A14-B6B4-DFDD1BBD70FC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -5486,12 +5495,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F61419B8-A98A-41CD-95EE-48A4F975B8D1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>